<commit_message>
Checksum and correct count
</commit_message>
<xml_diff>
--- a/ES-64 V2.xlsx
+++ b/ES-64 V2.xlsx
@@ -16,7 +16,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="341">
+  <si>
+    <t>CFR src</t>
+  </si>
   <si>
     <t>bits</t>
   </si>
@@ -24,21 +27,45 @@
     <t>D (dst\src)</t>
   </si>
   <si>
-    <t>CFR src</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
     <t>Big Endian Network Order</t>
   </si>
   <si>
+    <t>PC vectors</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>An</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
     <t>primary op</t>
   </si>
   <si>
+    <t>RP</t>
+  </si>
+  <si>
+    <t>halves</t>
+  </si>
+  <si>
     <t>An carries</t>
   </si>
   <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>BRK</t>
+  </si>
+  <si>
+    <t>Reserved</t>
+  </si>
+  <si>
     <t>dest Addr mode</t>
   </si>
   <si>
@@ -48,6 +75,9 @@
     <t>dest reg</t>
   </si>
   <si>
+    <t>Reg used as tertiary select operation</t>
+  </si>
+  <si>
     <t>secondary op</t>
   </si>
   <si>
@@ -57,6 +87,9 @@
     <t>Double(1)/Float(0) Default is D</t>
   </si>
   <si>
+    <t>Reserved extension opcodes</t>
+  </si>
+  <si>
     <t>size</t>
   </si>
   <si>
@@ -66,37 +99,28 @@
     <t>src Addr mode</t>
   </si>
   <si>
-    <t>PC vectors</t>
-  </si>
-  <si>
-    <t>IP</t>
-  </si>
-  <si>
-    <t>SP</t>
-  </si>
-  <si>
-    <t>RP</t>
-  </si>
-  <si>
-    <t>PC</t>
-  </si>
-  <si>
-    <t>BRK</t>
-  </si>
-  <si>
-    <t>Reserved</t>
-  </si>
-  <si>
     <t>0 equals 32</t>
   </si>
   <si>
+    <t>TRP</t>
+  </si>
+  <si>
+    <t>system design</t>
+  </si>
+  <si>
+    <t>Dn</t>
+  </si>
+  <si>
+    <t>fulls</t>
+  </si>
+  <si>
     <t>src reg</t>
   </si>
   <si>
     <t>quick</t>
   </si>
   <si>
-    <t>Reserved extension opcodes</t>
+    <t>8 * 8 = 64</t>
   </si>
   <si>
     <t>branch signed from PC+1</t>
@@ -105,78 +129,183 @@
     <t>Addr mode</t>
   </si>
   <si>
+    <t>HPR (P)</t>
+  </si>
+  <si>
+    <t>supervisor (P)</t>
+  </si>
+  <si>
     <t>#00</t>
   </si>
   <si>
-    <t>An</t>
+    <t>CIV (H)</t>
   </si>
   <si>
     <t>Not CFR src</t>
   </si>
   <si>
+    <t>hypervisor (H)</t>
+  </si>
+  <si>
+    <t>PCX</t>
+  </si>
+  <si>
+    <t>fast exchange</t>
+  </si>
+  <si>
     <t>.W</t>
   </si>
   <si>
+    <t>F</t>
+  </si>
+  <si>
     <t>#01</t>
   </si>
   <si>
     <t>(An)</t>
   </si>
   <si>
+    <t>IPX</t>
+  </si>
+  <si>
     <t>.L</t>
   </si>
   <si>
+    <t>of registers</t>
+  </si>
+  <si>
+    <t>COM (0 to 31)</t>
+  </si>
+  <si>
+    <t>User opcode</t>
+  </si>
+  <si>
     <t>#10</t>
   </si>
   <si>
-    <t>Dn</t>
+    <t>Reserved vector prefix opcodes</t>
   </si>
   <si>
     <t>.Q</t>
   </si>
   <si>
+    <t>compressed</t>
+  </si>
+  <si>
     <t>#11</t>
   </si>
   <si>
+    <t>SPX</t>
+  </si>
+  <si>
     <t>Special</t>
   </si>
   <si>
+    <t>improves code</t>
+  </si>
+  <si>
+    <t>extensions</t>
+  </si>
+  <si>
     <t>.D/.F</t>
   </si>
   <si>
+    <t>RPX</t>
+  </si>
+  <si>
+    <t>good stuff</t>
+  </si>
+  <si>
     <t>#000</t>
   </si>
   <si>
+    <t>pair</t>
+  </si>
+  <si>
+    <t>eval as nop</t>
+  </si>
+  <si>
     <t>Not float</t>
   </si>
   <si>
+    <t>The src MUST be an address for CFR to be CFR</t>
+  </si>
+  <si>
     <t>#001</t>
   </si>
   <si>
     <t>(PC+)/(-SP)</t>
   </si>
   <si>
+    <t>if not used (32)</t>
+  </si>
+  <si>
     <t>special write</t>
   </si>
   <si>
+    <t>halves An</t>
+  </si>
+  <si>
+    <t>Blocks of 8</t>
+  </si>
+  <si>
+    <t>B,W,L = half</t>
+  </si>
+  <si>
+    <t>register D</t>
+  </si>
+  <si>
+    <t>EXH</t>
+  </si>
+  <si>
+    <t>Exchange halves</t>
+  </si>
+  <si>
     <t>For PCX subroutine</t>
   </si>
   <si>
+    <t>is src</t>
+  </si>
+  <si>
+    <t>SXL</t>
+  </si>
+  <si>
     <t>#010</t>
   </si>
   <si>
+    <t>Sign extend low</t>
+  </si>
+  <si>
+    <t>FCN (float constant) not branches</t>
+  </si>
+  <si>
+    <t>INU</t>
+  </si>
+  <si>
     <t>#011</t>
   </si>
   <si>
+    <t>Increase upper</t>
+  </si>
+  <si>
     <t>(IP+)/(-RP)</t>
   </si>
   <si>
     <t>For IPX threaded code</t>
   </si>
   <si>
+    <t>DCU</t>
+  </si>
+  <si>
+    <t>Decrease upper</t>
+  </si>
+  <si>
     <t>#100</t>
   </si>
   <si>
+    <t>is dest</t>
+  </si>
+  <si>
     <t>#101</t>
   </si>
   <si>
@@ -198,12 +327,27 @@
     <t>D</t>
   </si>
   <si>
-    <t>F</t>
+    <t>@BRK</t>
+  </si>
+  <si>
+    <t>@TRP (P)</t>
+  </si>
+  <si>
+    <t>@HVR (H)</t>
+  </si>
+  <si>
+    <t>@CIV (H)</t>
+  </si>
+  <si>
+    <t>Set d64</t>
   </si>
   <si>
     <t>MOV</t>
   </si>
   <si>
+    <t>register F</t>
+  </si>
+  <si>
     <t>No dest read</t>
   </si>
   <si>
@@ -222,19 +366,22 @@
     <t>unsigned 5 bit</t>
   </si>
   <si>
-    <t>halves</t>
-  </si>
-  <si>
-    <t>Reg used as tertiary select operation</t>
-  </si>
-  <si>
-    <t>TRP</t>
-  </si>
-  <si>
-    <t>system design</t>
-  </si>
-  <si>
-    <t>8 * 8 = 64</t>
+    <t>SLT</t>
+  </si>
+  <si>
+    <t>Shift left Q half</t>
+  </si>
+  <si>
+    <t>SRT</t>
+  </si>
+  <si>
+    <t>Shift right Q half</t>
+  </si>
+  <si>
+    <t>ADU</t>
+  </si>
+  <si>
+    <t>Add upper</t>
   </si>
   <si>
     <t>MLL</t>
@@ -249,33 +396,63 @@
     <t>for compact</t>
   </si>
   <si>
+    <t>SBU</t>
+  </si>
+  <si>
+    <t>Subtract upper</t>
+  </si>
+  <si>
     <t>SUB</t>
   </si>
   <si>
     <t>SBQ</t>
   </si>
   <si>
+    <t>fulls Dn</t>
+  </si>
+  <si>
     <t>code</t>
   </si>
   <si>
+    <t>@COM</t>
+  </si>
+  <si>
     <t>CFR (specials)</t>
   </si>
   <si>
+    <t>W,L,Q</t>
+  </si>
+  <si>
     <t>BPL</t>
   </si>
   <si>
     <t>quick branch</t>
   </si>
   <si>
+    <t>ABS</t>
+  </si>
+  <si>
+    <t>Absolute</t>
+  </si>
+  <si>
     <t>AND</t>
   </si>
   <si>
     <t>BMI</t>
   </si>
   <si>
+    <t>Set d32</t>
+  </si>
+  <si>
     <t>0 and -1 do sign</t>
   </si>
   <si>
+    <t>SGN</t>
+  </si>
+  <si>
+    <t>Sign to 0 or -1</t>
+  </si>
+  <si>
     <t>ORR</t>
   </si>
   <si>
@@ -285,285 +462,261 @@
     <t xml:space="preserve">of 16 bit </t>
   </si>
   <si>
+    <t>SNP</t>
+  </si>
+  <si>
+    <t>NOT</t>
+  </si>
+  <si>
+    <t>super nop</t>
+  </si>
+  <si>
+    <t>Not</t>
+  </si>
+  <si>
+    <t>HNP</t>
+  </si>
+  <si>
+    <t>hyper nop</t>
+  </si>
+  <si>
     <t>XOR</t>
   </si>
   <si>
     <t>BNZ</t>
   </si>
   <si>
+    <t>CPL</t>
+  </si>
+  <si>
+    <t>SUP</t>
+  </si>
+  <si>
+    <t>Complement</t>
+  </si>
+  <si>
+    <t>set user PT d64</t>
+  </si>
+  <si>
+    <t>SSP</t>
+  </si>
+  <si>
+    <t>set super PT d64</t>
+  </si>
+  <si>
+    <t>WTO (group)</t>
+  </si>
+  <si>
+    <t>Write target override</t>
+  </si>
+  <si>
     <t>displacement</t>
   </si>
   <si>
+    <t>LSB</t>
+  </si>
+  <si>
+    <t>least significant bit (modulo 2)</t>
+  </si>
+  <si>
+    <t>ASR</t>
+  </si>
+  <si>
+    <t>Arith shift right</t>
+  </si>
+  <si>
     <t>D/F ops (size)</t>
   </si>
   <si>
+    <t>EIN</t>
+  </si>
+  <si>
     <t>D/F</t>
   </si>
   <si>
+    <t>enable interrupt</t>
+  </si>
+  <si>
+    <t>EVM</t>
+  </si>
+  <si>
+    <t>enable virt mem</t>
+  </si>
+  <si>
+    <t>LSR</t>
+  </si>
+  <si>
+    <t>Logic shift right</t>
+  </si>
+  <si>
     <t>FDV</t>
   </si>
   <si>
     <t>Divide</t>
   </si>
   <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>DIN</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>disable interrupt</t>
+  </si>
+  <si>
+    <t>DVM</t>
+  </si>
+  <si>
+    <t>WTO group</t>
+  </si>
+  <si>
     <t>FAD</t>
   </si>
   <si>
-    <t>fulls</t>
+    <t>UCC</t>
+  </si>
+  <si>
+    <t>disable virt mem</t>
   </si>
   <si>
     <t>FML</t>
   </si>
   <si>
+    <t>WTI</t>
+  </si>
+  <si>
+    <t>await interrupt</t>
+  </si>
+  <si>
+    <t>UCE</t>
+  </si>
+  <si>
+    <t>WTO</t>
+  </si>
+  <si>
     <t>FSB</t>
   </si>
   <si>
+    <t>CLI</t>
+  </si>
+  <si>
+    <t>clear interrupt</t>
+  </si>
+  <si>
+    <t>CLS</t>
+  </si>
+  <si>
+    <t>clear supervisor</t>
+  </si>
+  <si>
+    <t>CLH</t>
+  </si>
+  <si>
+    <t>clear hypervisor</t>
+  </si>
+  <si>
+    <t>RSS</t>
+  </si>
+  <si>
+    <t>reset super</t>
+  </si>
+  <si>
+    <t>RSH</t>
+  </si>
+  <si>
+    <t>reset hyper</t>
+  </si>
+  <si>
     <t>FBP</t>
   </si>
   <si>
+    <t>SIL</t>
+  </si>
+  <si>
+    <t>illegal super</t>
+  </si>
+  <si>
+    <t>HIL</t>
+  </si>
+  <si>
     <t>FBM</t>
   </si>
   <si>
+    <t>illegal hyper</t>
+  </si>
+  <si>
     <t>0 and 1 do sign</t>
   </si>
   <si>
+    <t>HPR is hypervisor trap</t>
+  </si>
+  <si>
     <t>FBD</t>
   </si>
   <si>
     <t>Branch denormal zero</t>
   </si>
   <si>
+    <t>BRK is user mode breakpoint trap</t>
+  </si>
+  <si>
     <t>FBI</t>
   </si>
   <si>
+    <t>WTO is set write target override for following instruction for 3 operands</t>
+  </si>
+  <si>
     <t>Branch infinity</t>
   </si>
   <si>
+    <t>CIV is set call interrupt vector (interrupt 0 is page fault)</t>
+  </si>
+  <si>
     <t>For efficient floats with own register set use vectors</t>
   </si>
   <si>
-    <t>PCX</t>
-  </si>
-  <si>
-    <t>fast exchange</t>
-  </si>
-  <si>
-    <t>IPX</t>
-  </si>
-  <si>
-    <t>of registers</t>
-  </si>
-  <si>
-    <t>SPX</t>
-  </si>
-  <si>
-    <t>improves code</t>
-  </si>
-  <si>
-    <t>RPX</t>
-  </si>
-  <si>
-    <t>good stuff</t>
-  </si>
-  <si>
-    <t>The src MUST be an address for CFR to be CFR</t>
-  </si>
-  <si>
-    <t>halves An</t>
-  </si>
-  <si>
-    <t>Blocks of 8</t>
-  </si>
-  <si>
-    <t>B,W,L = half</t>
-  </si>
-  <si>
-    <t>EXH</t>
-  </si>
-  <si>
-    <t>Exchange halves</t>
-  </si>
-  <si>
-    <t>SXL</t>
-  </si>
-  <si>
-    <t>Sign extend low</t>
-  </si>
-  <si>
-    <t>INU</t>
-  </si>
-  <si>
-    <t>Increase upper</t>
-  </si>
-  <si>
-    <t>DCU</t>
-  </si>
-  <si>
-    <t>Decrease upper</t>
-  </si>
-  <si>
-    <t>SLT</t>
-  </si>
-  <si>
-    <t>Shift left Q half</t>
-  </si>
-  <si>
-    <t>SRT</t>
-  </si>
-  <si>
-    <t>Shift right Q half</t>
-  </si>
-  <si>
-    <t>ADU</t>
-  </si>
-  <si>
-    <t>HPR (P)</t>
-  </si>
-  <si>
-    <t>Add upper</t>
-  </si>
-  <si>
-    <t>supervisor (P)</t>
-  </si>
-  <si>
-    <t>SBU</t>
-  </si>
-  <si>
-    <t>Subtract upper</t>
-  </si>
-  <si>
-    <t>CIV (H)</t>
-  </si>
-  <si>
-    <t>hypervisor (H)</t>
-  </si>
-  <si>
-    <t>fulls Dn</t>
-  </si>
-  <si>
-    <t>W,L,Q</t>
-  </si>
-  <si>
-    <t>ABS</t>
-  </si>
-  <si>
-    <t>Absolute</t>
-  </si>
-  <si>
-    <t>COM (0 to 31)</t>
-  </si>
-  <si>
-    <t>User opcode</t>
-  </si>
-  <si>
-    <t>SGN</t>
-  </si>
-  <si>
-    <t>Sign to 0 or -1</t>
-  </si>
-  <si>
-    <t>Reserved vector prefix opcodes</t>
-  </si>
-  <si>
-    <t>NOT</t>
-  </si>
-  <si>
-    <t>Not</t>
-  </si>
-  <si>
-    <t>CPL</t>
-  </si>
-  <si>
-    <t>compressed</t>
-  </si>
-  <si>
-    <t>Complement</t>
-  </si>
-  <si>
-    <t>extensions</t>
-  </si>
-  <si>
-    <t>WTO (group)</t>
-  </si>
-  <si>
-    <t>Write target override</t>
-  </si>
-  <si>
-    <t>LSB</t>
-  </si>
-  <si>
-    <t>least significant bit (modulo 2)</t>
-  </si>
-  <si>
-    <t>ASR</t>
-  </si>
-  <si>
-    <t>pair</t>
-  </si>
-  <si>
-    <t>Arith shift right</t>
-  </si>
-  <si>
-    <t>eval as nop</t>
-  </si>
-  <si>
-    <t>LSR</t>
-  </si>
-  <si>
-    <t>Logic shift right</t>
-  </si>
-  <si>
-    <t>if not used (32)</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>Q</t>
-  </si>
-  <si>
-    <t>register D</t>
-  </si>
-  <si>
-    <t>WTO group</t>
-  </si>
-  <si>
-    <t>UCC</t>
-  </si>
-  <si>
-    <t>is src</t>
-  </si>
-  <si>
-    <t>FCN (float constant) not branches</t>
-  </si>
-  <si>
-    <t>UCE</t>
-  </si>
-  <si>
-    <t>WTO</t>
-  </si>
-  <si>
-    <t>WTO is set write target override for following instruction for 3 operands</t>
+    <t>SUP and SSP followed by d64 immediate</t>
   </si>
   <si>
     <t>Only affects following instruction if at all</t>
   </si>
   <si>
+    <t>COM instruction pairs last can be tail recursive</t>
+  </si>
+  <si>
     <t>When used with MOV, MVQ, CFR but not specials except WTO makes a reserved nop pair</t>
   </si>
   <si>
+    <t>COM first can not be</t>
+  </si>
+  <si>
+    <t>This makes (@COM n COM m d16) a spare opcode space</t>
+  </si>
+  <si>
     <t>These reserved nop pairs may be assigned other function</t>
   </si>
   <si>
     <t>UCC is Unicode compress. W to a L with or joining for surrogate half</t>
   </si>
   <si>
+    <t>@ opcodes can't use PC, IP, SP, RP as src</t>
+  </si>
+  <si>
     <t>UCE is Unicode expand. L to a W with bit 27 set to make hi surrogate</t>
   </si>
   <si>
+    <t>WTO makes all these nop pairs</t>
+  </si>
+  <si>
+    <t>Only 32 float/double constants like pi</t>
+  </si>
+  <si>
     <t>WTO a MOV c,b becomes a = b/c for example</t>
   </si>
   <si>
@@ -576,33 +729,12 @@
     <t>DVQ</t>
   </si>
   <si>
-    <t>is dest</t>
-  </si>
-  <si>
-    <t>@BRK</t>
-  </si>
-  <si>
-    <t>@TRP (P)</t>
-  </si>
-  <si>
-    <t>@HVR (H)</t>
-  </si>
-  <si>
-    <t>@CIV (H)</t>
-  </si>
-  <si>
     <t>WTO branch becomes conditional register load with address (overrides PC write)</t>
   </si>
   <si>
-    <t>Set d64</t>
-  </si>
-  <si>
     <t>WTO then</t>
   </si>
   <si>
-    <t>register F</t>
-  </si>
-  <si>
     <t>CFR</t>
   </si>
   <si>
@@ -612,141 +744,63 @@
     <t>Get translated address</t>
   </si>
   <si>
-    <t>@COM</t>
-  </si>
-  <si>
-    <t>48 bit nop?</t>
-  </si>
-  <si>
-    <t>Set d32</t>
-  </si>
-  <si>
-    <t>SNP</t>
-  </si>
-  <si>
-    <t>super nop</t>
-  </si>
-  <si>
-    <t>HNP</t>
-  </si>
-  <si>
-    <t>hyper nop</t>
-  </si>
-  <si>
-    <t>SUP</t>
-  </si>
-  <si>
-    <t>set user PT d64</t>
-  </si>
-  <si>
-    <t>SSP</t>
-  </si>
-  <si>
-    <t>set super PT d64</t>
-  </si>
-  <si>
-    <t>EIN</t>
-  </si>
-  <si>
-    <t>enable interrupt</t>
-  </si>
-  <si>
-    <t>EVM</t>
-  </si>
-  <si>
-    <t>enable virt mem</t>
-  </si>
-  <si>
-    <t>DIN</t>
-  </si>
-  <si>
-    <t>disable interrupt</t>
-  </si>
-  <si>
-    <t>DVM</t>
-  </si>
-  <si>
-    <t>disable virt mem</t>
-  </si>
-  <si>
-    <t>WTI</t>
-  </si>
-  <si>
-    <t>await interrupt</t>
-  </si>
-  <si>
-    <t>CLI</t>
-  </si>
-  <si>
-    <t>clear interrupt</t>
-  </si>
-  <si>
-    <t>CLS</t>
-  </si>
-  <si>
-    <t>clear supervisor</t>
-  </si>
-  <si>
-    <t>CLH</t>
-  </si>
-  <si>
-    <t>clear hypervisor</t>
-  </si>
-  <si>
-    <t>RSS</t>
-  </si>
-  <si>
-    <t>reset super</t>
-  </si>
-  <si>
-    <t>RSH</t>
-  </si>
-  <si>
-    <t>reset hyper</t>
-  </si>
-  <si>
-    <t>SIL</t>
-  </si>
-  <si>
-    <t>illegal super</t>
-  </si>
-  <si>
-    <t>HIL</t>
-  </si>
-  <si>
-    <t>illegal hyper</t>
-  </si>
-  <si>
-    <t>HPR is hypervisor trap</t>
-  </si>
-  <si>
-    <t>BRK is user mode breakpoint trap</t>
-  </si>
-  <si>
-    <t>CIV is set call interrupt vector (interrupt 0 is page fault)</t>
-  </si>
-  <si>
-    <t>SUP and SSP followed by d64 immediate</t>
-  </si>
-  <si>
-    <t>COM instruction pairs last can be tail recursive</t>
-  </si>
-  <si>
-    <t>COM first can not be</t>
-  </si>
-  <si>
-    <t>This makes (@COM n COM m d16) a spare opcode space</t>
-  </si>
-  <si>
-    <t>@ opcodes can't use PC, IP, SP, RP as src</t>
-  </si>
-  <si>
-    <t>WTO makes all these nop pairs</t>
+    <t>CSM</t>
+  </si>
+  <si>
+    <t>Checksum check CSM keyexpect,delta</t>
+  </si>
+  <si>
+    <t>CSM is an execution checksum calculated and acted upon</t>
+  </si>
+  <si>
+    <t>The keyexpect can be put south of the checked code nesting include of check ok routine</t>
+  </si>
+  <si>
+    <t>As can be CPU ID specific can make code for CPU dependent on CPU</t>
+  </si>
+  <si>
+    <t>Check sum garuntee of execution and delta of last as initial post CSM</t>
+  </si>
+  <si>
+    <t>A checksum watchdog might be useful</t>
+  </si>
+  <si>
+    <t>NOP stability code watermark set</t>
+  </si>
+  <si>
+    <t>src,dst</t>
+  </si>
+  <si>
+    <t>PC,PC</t>
+  </si>
+  <si>
+    <t>PC,other</t>
+  </si>
+  <si>
+    <t>other,PC</t>
+  </si>
+  <si>
+    <t>WRP</t>
+  </si>
+  <si>
+    <t>ONG</t>
+  </si>
+  <si>
+    <t>RDP</t>
+  </si>
+  <si>
+    <t>RDP as left</t>
   </si>
   <si>
     <t xml:space="preserve"> (@COM n (COM m d16)) spare opcode space</t>
   </si>
   <si>
+    <t>All evaluate as nop unless assigned</t>
+  </si>
+  <si>
+    <t>Possible extension opcodes * sizes</t>
+  </si>
+  <si>
     <t>#nnn11nn0 011sssss opcode form points to</t>
   </si>
   <si>
@@ -762,12 +816,18 @@
     <t xml:space="preserve">Only first of pair, branches delay second as delay slot. </t>
   </si>
   <si>
+    <t>16 bit</t>
+  </si>
+  <si>
     <t>Second after branch may or may not speculative execute and commit</t>
   </si>
   <si>
     <t>Allow setting up and special COM?</t>
   </si>
   <si>
+    <t>Add in WTO any nop pair versions</t>
+  </si>
+  <si>
     <t>is the instruction replaced by profile COM</t>
   </si>
   <si>
@@ -792,9 +852,18 @@
     <t>(BRK/TRP/HPR/CIV m d16) spare opcode space</t>
   </si>
   <si>
+    <t>16 bit + 32 bit</t>
+  </si>
+  <si>
     <t>#mmm11mm0 111000</t>
   </si>
   <si>
+    <t>And WTO any for D/F with PC, IP, SP, RP</t>
+  </si>
+  <si>
+    <t>D16</t>
+  </si>
+  <si>
     <t>Except when mm is PC nnn is register special below</t>
   </si>
   <si>
@@ -819,6 +888,9 @@
     <t>Branch hit count since on</t>
   </si>
   <si>
+    <t>F16</t>
+  </si>
+  <si>
     <t>Data cache miss since on</t>
   </si>
   <si>
@@ -831,22 +903,13 @@
     <t>The register specials are only cleared via power cycle</t>
   </si>
   <si>
-    <t>NOP stability code watermark set</t>
-  </si>
-  <si>
-    <t>src,dst</t>
-  </si>
-  <si>
-    <t>PC,PC</t>
-  </si>
-  <si>
-    <t>PC,other</t>
-  </si>
-  <si>
-    <t>other,PC</t>
-  </si>
-  <si>
-    <t>WRP</t>
+    <t>DS4</t>
+  </si>
+  <si>
+    <t>DD4</t>
+  </si>
+  <si>
+    <t>FS4</t>
   </si>
   <si>
     <t>There are many other nops. Mainly on src,dest choices</t>
@@ -861,6 +924,9 @@
     <t>Excluding the above 2 all parameterized nops are not reserved</t>
   </si>
   <si>
+    <t>FD4</t>
+  </si>
+  <si>
     <t>They remain as power crypto differential nop tools and could assist automated coding</t>
   </si>
   <si>
@@ -903,27 +969,57 @@
     <t>Write Dst Commit</t>
   </si>
   <si>
-    <t>ONG</t>
-  </si>
-  <si>
-    <t>RDP</t>
+    <t>Reg - 4</t>
   </si>
   <si>
     <t>nop</t>
   </si>
   <si>
+    <t>OPs per block</t>
+  </si>
+  <si>
     <t>INS</t>
   </si>
   <si>
+    <t>Opcode prefixes</t>
+  </si>
+  <si>
+    <t>Excludes some WTO PC int and WTO PC,IP,SP,RP float-double</t>
+  </si>
+  <si>
+    <t>Still nops</t>
+  </si>
+  <si>
+    <t>All these express as reserved double nops</t>
+  </si>
+  <si>
+    <t>All on this page are reserved</t>
+  </si>
+  <si>
     <t>R2S+ (nop?)</t>
   </si>
   <si>
     <t>X1-</t>
   </si>
   <si>
+    <t>WRP is write prefix WRP d16 as nop unless used for d16 needing xtra write location</t>
+  </si>
+  <si>
+    <t>RDP d16 as nop unless used for d16 needing extra read</t>
+  </si>
+  <si>
+    <t>WTO RDP d16 is valid if d16 has alternate write target</t>
+  </si>
+  <si>
     <t>R2D+</t>
   </si>
   <si>
+    <t>RDP WTO is nop as WTO will be d16 yet to be defined</t>
+  </si>
+  <si>
+    <t>ONG is on goto for dense modulo switch jumps following instruction, zero based</t>
+  </si>
+  <si>
     <t>W1 (pass back)</t>
   </si>
   <si>
@@ -943,91 +1039,13 @@
   </si>
   <si>
     <t>Red box potential sum zero pre post</t>
-  </si>
-  <si>
-    <t>All evaluate as nop unless assigned</t>
-  </si>
-  <si>
-    <t>Possible extension opcodes * sizes</t>
-  </si>
-  <si>
-    <t>16 bit</t>
-  </si>
-  <si>
-    <t>Add in WTO any nop pair versions</t>
-  </si>
-  <si>
-    <t>16 bit + 32 bit</t>
-  </si>
-  <si>
-    <t>And WTO any for D/F with PC, IP, SP, RP</t>
-  </si>
-  <si>
-    <t>D16</t>
-  </si>
-  <si>
-    <t>F16</t>
-  </si>
-  <si>
-    <t>DS4</t>
-  </si>
-  <si>
-    <t>DD4</t>
-  </si>
-  <si>
-    <t>FS4</t>
-  </si>
-  <si>
-    <t>FD4</t>
-  </si>
-  <si>
-    <t>Reg - 4</t>
-  </si>
-  <si>
-    <t>OPs per block</t>
-  </si>
-  <si>
-    <t>Opcode prefixes</t>
-  </si>
-  <si>
-    <t>Excludes some WTO PC int and WTO PC,IP,SP,RP float-double</t>
-  </si>
-  <si>
-    <t>Still nops</t>
-  </si>
-  <si>
-    <t>All these express as reserved double nops</t>
-  </si>
-  <si>
-    <t>Plus 48 bit WTO WTO op</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>All on this page are reserved</t>
-  </si>
-  <si>
-    <t>WRP is write prefix WRP d16 as nop unless used for d16 needing xtra write location</t>
-  </si>
-  <si>
-    <t>RDP d16 as nop unless used for d16 needing extra read</t>
-  </si>
-  <si>
-    <t>WTO RDP d16 is valid if d16 has alternate write target</t>
-  </si>
-  <si>
-    <t>RDP WTO is nop as WTO will be d16 yet to be defined</t>
-  </si>
-  <si>
-    <t>ONG is on goto for dense modulo switch jumps following instruction, zero based</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1036,6 +1054,9 @@
     <font/>
     <font>
       <b/>
+    </font>
+    <font>
+      <color rgb="FFFF0000"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1063,34 +1084,9 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFF0000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFF0000"/>
-      </bottom>
     </border>
     <border>
       <top style="thin">
@@ -1103,20 +1099,23 @@
       </left>
     </border>
     <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-    </border>
-    <border>
-      <right style="thin">
+      <bottom style="thin">
         <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -1140,22 +1139,30 @@
       </bottom>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFFF0000"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFFF0000"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFFF0000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFFF0000"/>
       </bottom>
     </border>
     <border>
@@ -1178,6 +1185,31 @@
       </bottom>
     </border>
     <border>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF0000FF"/>
       </left>
@@ -1187,17 +1219,6 @@
       <top style="thin">
         <color rgb="FF0000FF"/>
       </top>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFF0000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFF0000"/>
-      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -1252,6 +1273,20 @@
       </bottom>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFFF00FF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF00FF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF00FF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF00FF"/>
+      </bottom>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FFFF0000"/>
       </right>
@@ -1267,25 +1302,11 @@
         <color rgb="FFFF0000"/>
       </bottom>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFF00FF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFF00FF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFF00FF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFF00FF"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1301,59 +1322,81 @@
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="18" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="19" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
     <xf borderId="20" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
     <xf borderId="21" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="22" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="23" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="24" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="25" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -1361,25 +1404,6 @@
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="23" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="24" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="25" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1424,7 +1448,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -1438,10 +1462,10 @@
         <v>3.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -1449,10 +1473,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
@@ -1460,7 +1484,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
@@ -1468,13 +1492,13 @@
         <v>1.0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
@@ -1482,10 +1506,10 @@
         <v>2.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
@@ -1493,13 +1517,13 @@
         <v>2.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C7" s="3">
         <v>5.0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8">
@@ -1507,418 +1531,418 @@
         <v>3.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>25</v>
+        <v>32</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>46</v>
+        <v>72</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>74</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>46</v>
+        <v>90</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>74</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>59</v>
+        <v>102</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>63</v>
+        <v>111</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>64</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>67</v>
+        <v>114</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>76</v>
+        <v>124</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>77</v>
+        <v>128</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>79</v>
+        <v>129</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>81</v>
+        <v>135</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>82</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>83</v>
+        <v>139</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>85</v>
+        <v>140</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>86</v>
+        <v>145</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>88</v>
+        <v>146</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>91</v>
+        <v>155</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>92</v>
+        <v>169</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>94</v>
+        <v>177</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>95</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>96</v>
+        <v>186</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>98</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>99</v>
+        <v>194</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>100</v>
+        <v>205</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>82</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>102</v>
+        <v>209</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>88</v>
+        <v>213</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>147</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>104</v>
+        <v>214</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>91</v>
+        <v>216</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>164</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>106</v>
+        <v>218</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>107</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -1938,390 +1962,415 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="10"/>
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
+        <v>31</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>109</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>111</v>
+        <v>49</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>113</v>
+        <v>59</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>115</v>
+        <v>64</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>117</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>118</v>
+        <v>76</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>119</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>120</v>
+        <v>79</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>121</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>122</v>
+        <v>83</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>123</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>124</v>
+        <v>87</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>118</v>
+        <v>76</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>149</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>155</v>
+        <v>94</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>162</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" s="1" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B34" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>174</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>175</v>
+        <v>185</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>176</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>177</v>
+        <v>222</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>178</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>180</v>
+        <v>228</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>181</v>
+        <v>230</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E43" s="19" t="s">
-        <v>183</v>
+        <v>233</v>
+      </c>
+      <c r="E43" s="22" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E44" s="21" t="s">
-        <v>185</v>
+        <v>235</v>
+      </c>
+      <c r="E44" s="24" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>191</v>
+        <v>237</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>193</v>
+        <v>238</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B48" s="22" t="s">
-        <v>196</v>
+        <v>239</v>
+      </c>
+      <c r="B48" s="25" t="s">
+        <v>240</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>197</v>
+        <v>241</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B49" s="19" t="s">
-        <v>22</v>
+        <v>193</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>242</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>199</v>
+        <v>243</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1"/>
-      <c r="B50" s="24"/>
+      <c r="B50" s="26"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="s">
+        <v>248</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2340,442 +2389,447 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="8"/>
+        <v>15</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" s="8"/>
+        <v>28</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="6"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>133</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="F4" s="8"/>
+        <v>38</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>138</v>
+        <v>40</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="8"/>
+        <v>42</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>144</v>
+        <v>52</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="E7" s="10"/>
+        <v>53</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="7"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="15"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="14"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="15"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="14"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="13"/>
+        <v>10</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="12"/>
     </row>
     <row r="11">
       <c r="A11" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>169</v>
+        <v>78</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="20"/>
+        <v>82</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>186</v>
+        <v>95</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>187</v>
+        <v>103</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>188</v>
+        <v>104</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>189</v>
+        <v>105</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>190</v>
+        <v>106</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>192</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>194</v>
+        <v>109</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="20"/>
+        <v>82</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="18"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="13"/>
+        <v>95</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12"/>
       <c r="F17" s="1" t="s">
-        <v>200</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>118</v>
+        <v>76</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>135</v>
+        <v>38</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>139</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>201</v>
+        <v>148</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>202</v>
+        <v>150</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>203</v>
+        <v>152</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>204</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>206</v>
+        <v>157</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>159</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="F21" s="20"/>
+        <v>160</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="F21" s="18"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>210</v>
+        <v>172</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>211</v>
+        <v>173</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>212</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>213</v>
+        <v>181</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>214</v>
+        <v>183</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>215</v>
+        <v>184</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>216</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>217</v>
+        <v>190</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>218</v>
+        <v>191</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>232</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>241</v>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="26"/>
-      <c r="B56" s="26"/>
-      <c r="C56" s="26"/>
+      <c r="A56" s="23"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2801,180 +2855,180 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>242</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>243</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>244</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>245</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>246</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>247</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>248</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>249</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>244</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>245</v>
+        <v>263</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>254</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>258</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>245</v>
+        <v>263</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>259</v>
+        <v>282</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>260</v>
+        <v>283</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>261</v>
+        <v>284</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>262</v>
+        <v>285</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>263</v>
+        <v>286</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>264</v>
+        <v>287</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>265</v>
+        <v>288</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>266</v>
+        <v>289</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>267</v>
+        <v>291</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>268</v>
+        <v>292</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>269</v>
+        <v>293</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>270</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -2994,7 +3048,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3003,64 +3057,72 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>273</v>
+        <v>251</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>274</v>
+        <v>252</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>275</v>
+        <v>253</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>276</v>
+        <v>254</v>
       </c>
       <c r="C3" s="28"/>
-      <c r="D3" s="30" t="s">
-        <v>295</v>
+      <c r="D3" s="29" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
+        <v>124</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="31" t="s">
+        <v>256</v>
+      </c>
       <c r="E4" s="27" t="s">
-        <v>296</v>
-      </c>
-      <c r="F4" s="14"/>
+        <v>257</v>
+      </c>
+      <c r="F4" s="10"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="E5" s="3">
-        <v>32.0</v>
+        <v>8.0</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" s="4">
-        <v>32.0</v>
+        <v>31</v>
+      </c>
+      <c r="E6" s="8">
+        <v>8.0</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>81</v>
+        <v>135</v>
       </c>
       <c r="E7" s="3">
         <v>32.0</v>
@@ -3068,74 +3130,74 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" s="9">
+        <v>140</v>
+      </c>
+      <c r="E8" s="13">
         <v>32.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" s="9">
+        <v>146</v>
+      </c>
+      <c r="E9" s="13">
         <v>32.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E10" s="4">
+        <v>155</v>
+      </c>
+      <c r="E10" s="8">
         <v>32.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" s="30">
+        <v>139</v>
+      </c>
+      <c r="B11" s="29">
         <v>1.0</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11" s="29">
         <v>31.0</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="29">
         <v>31.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" s="30">
+        <v>145</v>
+      </c>
+      <c r="B12" s="29">
         <v>1.0</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="29">
         <v>31.0</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="29">
         <v>31.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B13" s="30">
+        <v>154</v>
+      </c>
+      <c r="B13" s="29">
         <v>1.0</v>
       </c>
-      <c r="C13" s="30">
+      <c r="C13" s="29">
         <v>31.0</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D13" s="29">
         <v>31.0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="38">
+      <c r="A15" s="32">
         <f>SUM(B15:F15)</f>
-        <v>381</v>
+        <v>333</v>
       </c>
       <c r="B15">
         <f t="shared" ref="B15:E15" si="1">SUM(B3:B13)</f>
@@ -3151,51 +3213,51 @@
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>192</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>309</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="D17" s="38">
+        <v>260</v>
+      </c>
+      <c r="D17" s="32">
         <f>A15*3</f>
-        <v>1143</v>
+        <v>999</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>311</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="D20" s="38">
+        <v>269</v>
+      </c>
+      <c r="D20" s="32">
         <f>33*D17</f>
-        <v>37719</v>
+        <v>32967</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>313</v>
+        <v>278</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>314</v>
+        <v>280</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>315</v>
+        <v>281</v>
       </c>
       <c r="B22" s="1">
         <v>16.0</v>
@@ -3204,14 +3266,14 @@
         <f>B30</f>
         <v>8</v>
       </c>
-      <c r="D22" s="39">
+      <c r="D22" s="33">
         <f t="shared" ref="D22:D27" si="2">B22*C22</f>
         <v>128</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>316</v>
+        <v>290</v>
       </c>
       <c r="B23" s="1">
         <v>16.0</v>
@@ -3220,14 +3282,14 @@
         <f>B30</f>
         <v>8</v>
       </c>
-      <c r="D23" s="40">
+      <c r="D23" s="34">
         <f t="shared" si="2"/>
         <v>128</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>317</v>
+        <v>295</v>
       </c>
       <c r="B24" s="1">
         <v>2.0</v>
@@ -3236,14 +3298,14 @@
         <f>B29*B30</f>
         <v>224</v>
       </c>
-      <c r="D24" s="40">
+      <c r="D24" s="34">
         <f t="shared" si="2"/>
         <v>448</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>318</v>
+        <v>296</v>
       </c>
       <c r="B25" s="1">
         <v>4.0</v>
@@ -3252,14 +3314,14 @@
         <f>B29*B30</f>
         <v>224</v>
       </c>
-      <c r="D25" s="40">
+      <c r="D25" s="34">
         <f t="shared" si="2"/>
         <v>896</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>319</v>
+        <v>297</v>
       </c>
       <c r="B26" s="1">
         <v>2.0</v>
@@ -3268,14 +3330,14 @@
         <f>B29*B30</f>
         <v>224</v>
       </c>
-      <c r="D26" s="40">
+      <c r="D26" s="34">
         <f t="shared" si="2"/>
         <v>448</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
       <c r="B27" s="1">
         <v>4.0</v>
@@ -3284,7 +3346,7 @@
         <f>B29*B30</f>
         <v>224</v>
       </c>
-      <c r="D27" s="41">
+      <c r="D27" s="35">
         <f t="shared" si="2"/>
         <v>896</v>
       </c>
@@ -3297,7 +3359,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B29" s="1">
         <v>28.0</v>
@@ -3305,55 +3367,47 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B30" s="1">
         <v>8.0</v>
       </c>
-      <c r="D30" s="38">
+      <c r="D30" s="32">
         <f>D28+D20</f>
-        <v>134871</v>
+        <v>130119</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>325</v>
+        <v>322</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="D35" s="38">
-        <f>D30+65536*32*32</f>
-        <v>67243735</v>
-      </c>
+      <c r="A35" s="16" t="s">
+        <v>325</v>
+      </c>
+      <c r="B35" s="18"/>
     </row>
     <row r="36">
-      <c r="C36" s="1" t="s">
+      <c r="A36" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D36">
-        <f>D35+D30</f>
-        <v>67378606</v>
-      </c>
     </row>
     <row r="37">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="B37" s="20"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
@@ -3362,27 +3416,17 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="1" t="s">
         <v>333</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="s">
-        <v>334</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A35:B35"/>
     <mergeCell ref="B3:C3"/>
   </mergeCells>
   <drawing r:id="rId1"/>
@@ -3401,220 +3445,220 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>277</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>278</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>279</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>280</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>281</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>130</v>
+        <v>304</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>118</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>283</v>
+        <v>305</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>285</v>
+        <v>306</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>307</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>286</v>
+        <v>308</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>287</v>
+        <v>309</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>288</v>
+        <v>310</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>289</v>
+        <v>311</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>290</v>
+        <v>312</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>291</v>
+        <v>313</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>293</v>
+        <v>315</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>294</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="29"/>
-      <c r="B14" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="10"/>
+      <c r="A14" s="36"/>
+      <c r="B14" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="7"/>
       <c r="F14" s="1" t="s">
-        <v>297</v>
+        <v>318</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="32" t="s">
-        <v>298</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13"/>
+      <c r="A15" s="37" t="s">
+        <v>320</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="12"/>
       <c r="F15" s="1" t="s">
-        <v>297</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="29"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="10"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="7"/>
       <c r="F16" s="1" t="s">
-        <v>297</v>
+        <v>318</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="11"/>
-      <c r="B17" s="33" t="s">
-        <v>298</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="13"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="38" t="s">
+        <v>320</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12"/>
       <c r="F17" s="1" t="s">
-        <v>299</v>
+        <v>326</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="29"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="34" t="s">
-        <v>300</v>
+      <c r="A18" s="36"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="39" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="33" t="s">
-        <v>298</v>
-      </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="35" t="s">
-        <v>301</v>
+      <c r="A19" s="9"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="38" t="s">
+        <v>320</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="40" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="29"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="36" t="s">
-        <v>175</v>
+      <c r="A20" s="36"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="41" t="s">
+        <v>193</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>302</v>
+        <v>334</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="33" t="s">
-        <v>298</v>
-      </c>
-      <c r="E21" s="13"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="38" t="s">
+        <v>320</v>
+      </c>
+      <c r="E21" s="12"/>
       <c r="F21" s="1" t="s">
-        <v>303</v>
+        <v>335</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="29"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="10"/>
+      <c r="A22" s="36"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="7"/>
       <c r="F22" s="1" t="s">
-        <v>297</v>
+        <v>318</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="11"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="37" t="s">
-        <v>298</v>
+      <c r="A23" s="9"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="42" t="s">
+        <v>320</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>304</v>
+        <v>336</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>305</v>
+        <v>337</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>306</v>
+        <v>338</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>307</v>
+        <v>339</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>308</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>